<commit_message>
Changed Database, updated case sensitive paths of images
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Javascript\Vers 4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848B9411-14AC-4BF4-9EB1-C18CC0B4186A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E89B07-FA4B-4EE4-9A61-5C407AEF93B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,9 +436,6 @@
     <t>  Earth is the third planet from the Sun and the only known planet to support life. It has a diverse environment with oceans, landmasses, and a breathable atmosphere, which is primarily composed of nitrogen and oxygen. Earth’s surface is constantly changing due to geological activity, and it is the only planet with liquid water on its surface, which is essential for life. The planet has one natural satellite, the Moon, which has a significant effect on Earth’s tides. Earth’s magnetic field protects it from solar and cosmic radiation, creating a stable environment for life to thrive.</t>
   </si>
   <si>
-    <t>Images/Earth.jpg</t>
-  </si>
-  <si>
     <t>Mass: 5.972 x 10^24 kg&lt;br&gt;Distance from Sun: 149.6 million km&lt;br&gt;Discovered: Known since Antiquity</t>
   </si>
   <si>
@@ -700,9 +697,6 @@
     <t>  TRAPPIST-1e is an exoplanet located about 40 light-years away in the constellation Aquarius. It is one of seven planets in the TRAPPIST-1 system, all of which are roughly the size of Earth and orbit a cool red dwarf star. TRAPPIST-1e is located in the habitable zone of its star, where liquid water could exist on its surface. This planet is considered one of the best candidates for the search for life beyond Earth, with a potentially Earth-like atmosphere and surface conditions.</t>
   </si>
   <si>
-    <t>Images/Trappist_1e.png</t>
-  </si>
-  <si>
     <t>Mass: ~0.92 x Earth&lt;br&gt;Distance from Earth: 40 light-years&lt;br&gt;Discovered: 2017</t>
   </si>
   <si>
@@ -712,9 +706,6 @@
     <t>  WASP-12b is an exoplanet located about 1,400 light-years away in the constellation Auriga. It is a gas giant with an unusual and extreme environment, orbiting very close to its parent star. The planet is tidally locked, meaning one side always faces the star, while the other side remains in perpetual darkness. The temperatures on the star-facing side of WASP-12b can reach up to 2,500°C (4,532°F), making it one of the hottest exoplanets known. Its extreme conditions provide valuable insights into the behavior of planets in close orbits.</t>
   </si>
   <si>
-    <t>Images/Wasp_12b.jpg</t>
-  </si>
-  <si>
     <t>Mass: 1.39 x Jupiter&lt;br&gt;Distance from Earth: 1400 light-years&lt;br&gt;Discovered: 2008</t>
   </si>
   <si>
@@ -736,9 +727,6 @@
     <t>  GJ 1132 b is an exoplanet located about 39 light-years away in the constellation Vela. It is one of the closest Earth-sized exoplanets and is classified as a "super-Earth" due to its mass being about 1.6 times that of Earth. The planet is rocky and has a thick atmosphere, which might be composed of hydrogen, methane, and water vapor. GJ 1132 b's atmosphere has been a subject of study, as it could offer clues about the potential habitability of planets beyond our solar system.</t>
   </si>
   <si>
-    <t>Images/GJ_1131_b.jpg</t>
-  </si>
-  <si>
     <t>Mass: ~1.6 x Earth&lt;br&gt;Distance from Earth: 39 light-years&lt;br&gt;Discovered: 2015</t>
   </si>
   <si>
@@ -1631,9 +1619,6 @@
   </si>
   <si>
     <t>XTE J1550-564 is a stellar-mass black hole located roughly 17,000 light-years away in the constellation Norma. Known for its X-ray flares and relativistic jets, it offers an excellent opportunity to study accretion physics and jet formation. This black hole is in a binary system with a low-mass companion star and has an estimated mass of about 10 solar masses. Its dramatic outbursts have provided valuable data for understanding black hole behavior and dynamics in binary systems.</t>
-  </si>
-  <si>
-    <t>Images/XTE_J1550_564.jpg</t>
   </si>
   <si>
     <t>Mass: ~10 solar masses&lt;br&gt;Distance: 12,000 light-years&lt;br&gt;Type: Stellar</t>
@@ -2117,6 +2102,21 @@
   <si>
     <t>Today is a day of inspiration and creativity for you, dear Pisces. You’ll find yourself brimming with ideas and a desire to express your emotions through creative outlets. Whether it’s writing, painting, cooking, or even problem-solving, let your imagination take the lead. Pay attention to the little things around you—they could spark your next great idea. &lt;br&gt;_x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D__x000D_
 Don’t be afraid to experiment and try new approaches, as this will only deepen your creative experience. Trust your intuition to guide you toward what feels right. By channeling your energy into artistic pursuits, you’ll not only find joy but also inspire those around you. Let today be a celebration of your unique ability to turn dreams into reality.</t>
+  </si>
+  <si>
+    <t>Images/TRAPPIST_1e.png</t>
+  </si>
+  <si>
+    <t>Images/Earth.JPG</t>
+  </si>
+  <si>
+    <t>Images/GJ_1131_b.JPG</t>
+  </si>
+  <si>
+    <t>Images/WASP_12b.jpg</t>
+  </si>
+  <si>
+    <t>Images/XTE_J1550_564.JPG</t>
   </si>
 </sst>
 </file>
@@ -2493,15 +2493,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152:XFD152"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>90</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>118</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>126</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>135</v>
       </c>
@@ -3070,2009 +3070,2008 @@
         <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>137</v>
+        <v>688</v>
       </c>
       <c r="D34" t="s">
         <v>129</v>
       </c>
       <c r="E34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>139</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>140</v>
-      </c>
-      <c r="C35" t="s">
-        <v>141</v>
       </c>
       <c r="D35" t="s">
         <v>129</v>
       </c>
       <c r="E35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
         <v>143</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>144</v>
-      </c>
-      <c r="C36" t="s">
-        <v>145</v>
       </c>
       <c r="D36" t="s">
         <v>129</v>
       </c>
       <c r="E36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>147</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>148</v>
-      </c>
-      <c r="C37" t="s">
-        <v>149</v>
       </c>
       <c r="D37" t="s">
         <v>129</v>
       </c>
       <c r="E37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>151</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>152</v>
-      </c>
-      <c r="C38" t="s">
-        <v>153</v>
       </c>
       <c r="D38" t="s">
         <v>129</v>
       </c>
       <c r="E38" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>155</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>156</v>
-      </c>
-      <c r="C39" t="s">
-        <v>157</v>
       </c>
       <c r="D39" t="s">
         <v>129</v>
       </c>
       <c r="E39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>159</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>160</v>
-      </c>
-      <c r="C40" t="s">
-        <v>161</v>
       </c>
       <c r="D40" t="s">
         <v>129</v>
       </c>
       <c r="E40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>163</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>164</v>
-      </c>
-      <c r="C41" t="s">
-        <v>165</v>
       </c>
       <c r="D41" t="s">
         <v>129</v>
       </c>
       <c r="E41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>167</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>168</v>
-      </c>
-      <c r="C42" t="s">
-        <v>169</v>
       </c>
       <c r="D42" t="s">
         <v>129</v>
       </c>
       <c r="E42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>171</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>172</v>
-      </c>
-      <c r="C43" t="s">
-        <v>173</v>
       </c>
       <c r="D43" t="s">
         <v>129</v>
       </c>
       <c r="E43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>175</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>176</v>
-      </c>
-      <c r="C44" t="s">
-        <v>177</v>
       </c>
       <c r="D44" t="s">
         <v>129</v>
       </c>
       <c r="E44" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>179</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>180</v>
-      </c>
-      <c r="C45" t="s">
-        <v>181</v>
       </c>
       <c r="D45" t="s">
         <v>129</v>
       </c>
       <c r="E45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>183</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>184</v>
-      </c>
-      <c r="C46" t="s">
-        <v>185</v>
       </c>
       <c r="D46" t="s">
         <v>129</v>
       </c>
       <c r="E46" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>187</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>188</v>
-      </c>
-      <c r="C47" t="s">
-        <v>189</v>
       </c>
       <c r="D47" t="s">
         <v>129</v>
       </c>
       <c r="E47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>191</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>192</v>
-      </c>
-      <c r="C48" t="s">
-        <v>193</v>
       </c>
       <c r="D48" t="s">
         <v>129</v>
       </c>
       <c r="E48" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
         <v>195</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>196</v>
-      </c>
-      <c r="C49" t="s">
-        <v>197</v>
       </c>
       <c r="D49" t="s">
         <v>129</v>
       </c>
       <c r="E49" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
         <v>199</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>200</v>
-      </c>
-      <c r="C50" t="s">
-        <v>201</v>
       </c>
       <c r="D50" t="s">
         <v>129</v>
       </c>
       <c r="E50" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>203</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>204</v>
-      </c>
-      <c r="C51" t="s">
-        <v>205</v>
       </c>
       <c r="D51" t="s">
         <v>129</v>
       </c>
       <c r="E51" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
         <v>207</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>208</v>
-      </c>
-      <c r="C52" t="s">
-        <v>209</v>
       </c>
       <c r="D52" t="s">
         <v>129</v>
       </c>
       <c r="E52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
         <v>211</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>212</v>
-      </c>
-      <c r="C53" t="s">
-        <v>213</v>
       </c>
       <c r="D53" t="s">
         <v>129</v>
       </c>
       <c r="E53" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
         <v>215</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>216</v>
-      </c>
-      <c r="C54" t="s">
-        <v>217</v>
       </c>
       <c r="D54" t="s">
         <v>129</v>
       </c>
       <c r="E54" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
         <v>219</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>220</v>
-      </c>
-      <c r="C55" t="s">
-        <v>221</v>
       </c>
       <c r="D55" t="s">
         <v>129</v>
       </c>
       <c r="E55" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
         <v>223</v>
       </c>
-      <c r="B56" t="s">
-        <v>224</v>
-      </c>
       <c r="C56" t="s">
-        <v>225</v>
+        <v>687</v>
       </c>
       <c r="D56" t="s">
         <v>129</v>
       </c>
       <c r="E56" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>225</v>
+      </c>
+      <c r="B57" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>227</v>
-      </c>
-      <c r="B57" t="s">
-        <v>228</v>
-      </c>
       <c r="C57" t="s">
-        <v>229</v>
+        <v>690</v>
       </c>
       <c r="D57" t="s">
         <v>129</v>
       </c>
       <c r="E57" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>228</v>
+      </c>
+      <c r="B58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C58" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>231</v>
-      </c>
-      <c r="B58" t="s">
-        <v>232</v>
-      </c>
-      <c r="C58" t="s">
-        <v>233</v>
       </c>
       <c r="D58" t="s">
         <v>129</v>
       </c>
       <c r="E58" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B59" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C59" t="s">
-        <v>237</v>
+        <v>689</v>
       </c>
       <c r="D59" t="s">
         <v>129</v>
       </c>
       <c r="E59" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B60" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C60" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D60" t="s">
         <v>129</v>
       </c>
       <c r="E60" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B61" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C61" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D61" t="s">
         <v>129</v>
       </c>
       <c r="E61" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>243</v>
+      </c>
+      <c r="B62" t="s">
+        <v>244</v>
+      </c>
+      <c r="C62" t="s">
+        <v>245</v>
+      </c>
+      <c r="D62" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+      <c r="E62" t="s">
         <v>247</v>
       </c>
-      <c r="B62" t="s">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>248</v>
       </c>
-      <c r="C62" t="s">
+      <c r="B63" t="s">
         <v>249</v>
       </c>
-      <c r="D62" t="s">
+      <c r="C63" t="s">
         <v>250</v>
       </c>
-      <c r="E62" t="s">
+      <c r="D63" t="s">
+        <v>246</v>
+      </c>
+      <c r="E63" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>252</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>253</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>254</v>
       </c>
-      <c r="D63" t="s">
-        <v>250</v>
-      </c>
-      <c r="E63" t="s">
+      <c r="D64" t="s">
+        <v>246</v>
+      </c>
+      <c r="E64" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>256</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>257</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>258</v>
       </c>
-      <c r="D64" t="s">
-        <v>250</v>
-      </c>
-      <c r="E64" t="s">
+      <c r="D65" t="s">
+        <v>246</v>
+      </c>
+      <c r="E65" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>260</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>261</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>262</v>
       </c>
-      <c r="D65" t="s">
-        <v>250</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="D66" t="s">
+        <v>246</v>
+      </c>
+      <c r="E66" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>264</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>265</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>266</v>
       </c>
-      <c r="D66" t="s">
-        <v>250</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="D67" t="s">
+        <v>246</v>
+      </c>
+      <c r="E67" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>268</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>269</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>270</v>
       </c>
-      <c r="D67" t="s">
-        <v>250</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="D68" t="s">
+        <v>246</v>
+      </c>
+      <c r="E68" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>272</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>273</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>274</v>
       </c>
-      <c r="D68" t="s">
-        <v>250</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D69" t="s">
+        <v>246</v>
+      </c>
+      <c r="E69" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>276</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>277</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>278</v>
       </c>
-      <c r="D69" t="s">
-        <v>250</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="D70" t="s">
+        <v>246</v>
+      </c>
+      <c r="E70" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>280</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>281</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>282</v>
       </c>
-      <c r="D70" t="s">
-        <v>250</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="D71" t="s">
+        <v>246</v>
+      </c>
+      <c r="E71" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>284</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>285</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>286</v>
       </c>
-      <c r="D71" t="s">
-        <v>250</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="D72" t="s">
+        <v>246</v>
+      </c>
+      <c r="E72" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>288</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>289</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>290</v>
       </c>
-      <c r="D72" t="s">
-        <v>250</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="D73" t="s">
+        <v>246</v>
+      </c>
+      <c r="E73" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>292</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>293</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>294</v>
       </c>
-      <c r="D73" t="s">
-        <v>250</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="D74" t="s">
+        <v>246</v>
+      </c>
+      <c r="E74" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>296</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>297</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>298</v>
       </c>
-      <c r="D74" t="s">
-        <v>250</v>
-      </c>
-      <c r="E74" t="s">
+      <c r="D75" t="s">
+        <v>246</v>
+      </c>
+      <c r="E75" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>300</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>301</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>302</v>
       </c>
-      <c r="D75" t="s">
-        <v>250</v>
-      </c>
-      <c r="E75" t="s">
+      <c r="D76" t="s">
+        <v>246</v>
+      </c>
+      <c r="E76" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>304</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>305</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>306</v>
       </c>
-      <c r="D76" t="s">
-        <v>250</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="D77" t="s">
+        <v>246</v>
+      </c>
+      <c r="E77" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>308</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>309</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>310</v>
       </c>
-      <c r="D77" t="s">
-        <v>250</v>
-      </c>
-      <c r="E77" t="s">
+      <c r="D78" t="s">
+        <v>246</v>
+      </c>
+      <c r="E78" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>312</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>313</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" t="s">
         <v>314</v>
       </c>
-      <c r="D78" t="s">
-        <v>250</v>
-      </c>
-      <c r="E78" t="s">
+      <c r="D79" t="s">
+        <v>246</v>
+      </c>
+      <c r="E79" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>316</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>317</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>318</v>
       </c>
-      <c r="D79" t="s">
-        <v>250</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="D80" t="s">
+        <v>246</v>
+      </c>
+      <c r="E80" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>320</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>321</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C81" t="s">
         <v>322</v>
       </c>
-      <c r="D80" t="s">
-        <v>250</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="D81" t="s">
+        <v>246</v>
+      </c>
+      <c r="E81" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>324</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>325</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" t="s">
         <v>326</v>
       </c>
-      <c r="D81" t="s">
-        <v>250</v>
-      </c>
-      <c r="E81" t="s">
+      <c r="D82" t="s">
+        <v>246</v>
+      </c>
+      <c r="E82" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>328</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>329</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>330</v>
       </c>
-      <c r="D82" t="s">
-        <v>250</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="D83" t="s">
+        <v>246</v>
+      </c>
+      <c r="E83" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>332</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>333</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>334</v>
       </c>
-      <c r="D83" t="s">
-        <v>250</v>
-      </c>
-      <c r="E83" t="s">
+      <c r="D84" t="s">
+        <v>246</v>
+      </c>
+      <c r="E84" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>336</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B85" t="s">
         <v>337</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>338</v>
       </c>
-      <c r="D84" t="s">
-        <v>250</v>
-      </c>
-      <c r="E84" t="s">
+      <c r="D85" t="s">
+        <v>246</v>
+      </c>
+      <c r="E85" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>340</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>341</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>342</v>
       </c>
-      <c r="D85" t="s">
-        <v>250</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="D86" t="s">
+        <v>246</v>
+      </c>
+      <c r="E86" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>344</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>345</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" t="s">
         <v>346</v>
       </c>
-      <c r="D86" t="s">
-        <v>250</v>
-      </c>
-      <c r="E86" t="s">
+      <c r="D87" t="s">
+        <v>246</v>
+      </c>
+      <c r="E87" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>348</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>349</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>350</v>
       </c>
-      <c r="D87" t="s">
-        <v>250</v>
-      </c>
-      <c r="E87" t="s">
+      <c r="D88" t="s">
+        <v>246</v>
+      </c>
+      <c r="E88" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>352</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" t="s">
         <v>353</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>354</v>
       </c>
-      <c r="D88" t="s">
-        <v>250</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="D89" t="s">
+        <v>246</v>
+      </c>
+      <c r="E89" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>356</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B90" t="s">
         <v>357</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>358</v>
       </c>
-      <c r="D89" t="s">
-        <v>250</v>
-      </c>
-      <c r="E89" t="s">
+      <c r="D90" t="s">
+        <v>246</v>
+      </c>
+      <c r="E90" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>360</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>361</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>362</v>
       </c>
-      <c r="D90" t="s">
-        <v>250</v>
-      </c>
-      <c r="E90" t="s">
+      <c r="D91" t="s">
+        <v>246</v>
+      </c>
+      <c r="E91" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>364</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>365</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
         <v>366</v>
       </c>
-      <c r="D91" t="s">
-        <v>250</v>
-      </c>
-      <c r="E91" t="s">
+      <c r="D92" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
+      <c r="E92" t="s">
         <v>368</v>
       </c>
-      <c r="B92" t="s">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>369</v>
       </c>
-      <c r="C92" t="s">
+      <c r="B93" t="s">
         <v>370</v>
       </c>
-      <c r="D92" t="s">
+      <c r="C93" t="s">
         <v>371</v>
       </c>
-      <c r="E92" t="s">
+      <c r="D93" t="s">
+        <v>367</v>
+      </c>
+      <c r="E93" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>373</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>374</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>375</v>
       </c>
-      <c r="D93" t="s">
-        <v>371</v>
-      </c>
-      <c r="E93" t="s">
+      <c r="D94" t="s">
+        <v>367</v>
+      </c>
+      <c r="E94" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>377</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B95" t="s">
         <v>378</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C95" t="s">
         <v>379</v>
       </c>
-      <c r="D94" t="s">
-        <v>371</v>
-      </c>
-      <c r="E94" t="s">
+      <c r="D95" t="s">
+        <v>367</v>
+      </c>
+      <c r="E95" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A95" t="s">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>381</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>382</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>383</v>
       </c>
-      <c r="D95" t="s">
-        <v>371</v>
-      </c>
-      <c r="E95" t="s">
+      <c r="D96" t="s">
+        <v>367</v>
+      </c>
+      <c r="E96" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>385</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>386</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>387</v>
       </c>
-      <c r="D96" t="s">
-        <v>371</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="D97" t="s">
+        <v>367</v>
+      </c>
+      <c r="E97" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>389</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>390</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C98" t="s">
         <v>391</v>
       </c>
-      <c r="D97" t="s">
-        <v>371</v>
-      </c>
-      <c r="E97" t="s">
+      <c r="D98" t="s">
+        <v>367</v>
+      </c>
+      <c r="E98" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>393</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>394</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>395</v>
       </c>
-      <c r="D98" t="s">
-        <v>371</v>
-      </c>
-      <c r="E98" t="s">
+      <c r="D99" t="s">
+        <v>367</v>
+      </c>
+      <c r="E99" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>397</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>398</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>399</v>
       </c>
-      <c r="D99" t="s">
-        <v>371</v>
-      </c>
-      <c r="E99" t="s">
+      <c r="D100" t="s">
+        <v>367</v>
+      </c>
+      <c r="E100" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A100" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>401</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>402</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>403</v>
       </c>
-      <c r="D100" t="s">
-        <v>371</v>
-      </c>
-      <c r="E100" t="s">
+      <c r="D101" t="s">
+        <v>367</v>
+      </c>
+      <c r="E101" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>405</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>406</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>407</v>
       </c>
-      <c r="D101" t="s">
-        <v>371</v>
-      </c>
-      <c r="E101" t="s">
+      <c r="D102" t="s">
+        <v>367</v>
+      </c>
+      <c r="E102" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>409</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>410</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C103" t="s">
         <v>411</v>
       </c>
-      <c r="D102" t="s">
-        <v>371</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="D103" t="s">
+        <v>367</v>
+      </c>
+      <c r="E103" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>413</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B104" t="s">
         <v>414</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>415</v>
       </c>
-      <c r="D103" t="s">
-        <v>371</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="D104" t="s">
+        <v>367</v>
+      </c>
+      <c r="E104" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>417</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>418</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C105" t="s">
         <v>419</v>
       </c>
-      <c r="D104" t="s">
-        <v>371</v>
-      </c>
-      <c r="E104" t="s">
+      <c r="D105" t="s">
+        <v>367</v>
+      </c>
+      <c r="E105" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>421</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>422</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>423</v>
       </c>
-      <c r="D105" t="s">
-        <v>371</v>
-      </c>
-      <c r="E105" t="s">
+      <c r="D106" t="s">
+        <v>367</v>
+      </c>
+      <c r="E106" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A106" t="s">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>425</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>426</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>427</v>
       </c>
-      <c r="D106" t="s">
-        <v>371</v>
-      </c>
-      <c r="E106" t="s">
+      <c r="D107" t="s">
+        <v>367</v>
+      </c>
+      <c r="E107" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>429</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>430</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>431</v>
       </c>
-      <c r="D107" t="s">
-        <v>371</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="D108" t="s">
+        <v>367</v>
+      </c>
+      <c r="E108" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A108" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>433</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>434</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C109" t="s">
         <v>435</v>
       </c>
-      <c r="D108" t="s">
-        <v>371</v>
-      </c>
-      <c r="E108" t="s">
+      <c r="D109" t="s">
+        <v>367</v>
+      </c>
+      <c r="E109" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>437</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>438</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>439</v>
       </c>
-      <c r="D109" t="s">
-        <v>371</v>
-      </c>
-      <c r="E109" t="s">
+      <c r="D110" t="s">
+        <v>367</v>
+      </c>
+      <c r="E110" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>441</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>442</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>443</v>
       </c>
-      <c r="D110" t="s">
-        <v>371</v>
-      </c>
-      <c r="E110" t="s">
+      <c r="D111" t="s">
+        <v>367</v>
+      </c>
+      <c r="E111" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>445</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B112" t="s">
         <v>446</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>447</v>
       </c>
-      <c r="D111" t="s">
-        <v>371</v>
-      </c>
-      <c r="E111" t="s">
+      <c r="D112" t="s">
+        <v>367</v>
+      </c>
+      <c r="E112" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>449</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>450</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C113" t="s">
         <v>451</v>
       </c>
-      <c r="D112" t="s">
-        <v>371</v>
-      </c>
-      <c r="E112" t="s">
+      <c r="D113" t="s">
+        <v>367</v>
+      </c>
+      <c r="E113" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>453</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>454</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>455</v>
       </c>
-      <c r="D113" t="s">
-        <v>371</v>
-      </c>
-      <c r="E113" t="s">
+      <c r="D114" t="s">
+        <v>367</v>
+      </c>
+      <c r="E114" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A114" t="s">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>457</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>458</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C115" t="s">
         <v>459</v>
       </c>
-      <c r="D114" t="s">
-        <v>371</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="D115" t="s">
+        <v>367</v>
+      </c>
+      <c r="E115" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>461</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>462</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C116" t="s">
         <v>463</v>
       </c>
-      <c r="D115" t="s">
-        <v>371</v>
-      </c>
-      <c r="E115" t="s">
+      <c r="D116" t="s">
+        <v>367</v>
+      </c>
+      <c r="E116" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>465</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>466</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>467</v>
       </c>
-      <c r="D116" t="s">
-        <v>371</v>
-      </c>
-      <c r="E116" t="s">
+      <c r="D117" t="s">
+        <v>367</v>
+      </c>
+      <c r="E117" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="117" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>469</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B118" t="s">
         <v>470</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C118" t="s">
         <v>471</v>
       </c>
-      <c r="D117" t="s">
-        <v>371</v>
-      </c>
-      <c r="E117" t="s">
+      <c r="D118" t="s">
+        <v>367</v>
+      </c>
+      <c r="E118" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A118" t="s">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>473</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B119" t="s">
         <v>474</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>475</v>
       </c>
-      <c r="D118" t="s">
-        <v>371</v>
-      </c>
-      <c r="E118" t="s">
+      <c r="D119" t="s">
+        <v>367</v>
+      </c>
+      <c r="E119" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A119" t="s">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>477</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>478</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C120" t="s">
         <v>479</v>
       </c>
-      <c r="D119" t="s">
-        <v>371</v>
-      </c>
-      <c r="E119" t="s">
+      <c r="D120" t="s">
+        <v>367</v>
+      </c>
+      <c r="E120" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A120" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>481</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B121" t="s">
         <v>482</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C121" t="s">
         <v>483</v>
       </c>
-      <c r="D120" t="s">
-        <v>371</v>
-      </c>
-      <c r="E120" t="s">
+      <c r="D121" t="s">
+        <v>367</v>
+      </c>
+      <c r="E121" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A121" t="s">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>485</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>486</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C122" t="s">
         <v>487</v>
       </c>
-      <c r="D121" t="s">
-        <v>371</v>
-      </c>
-      <c r="E121" t="s">
+      <c r="D122" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
+      <c r="E122" t="s">
         <v>489</v>
       </c>
-      <c r="B122" t="s">
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>490</v>
       </c>
-      <c r="C122" t="s">
+      <c r="B123" t="s">
         <v>491</v>
       </c>
-      <c r="D122" t="s">
+      <c r="C123" t="s">
         <v>492</v>
       </c>
-      <c r="E122" t="s">
+      <c r="D123" t="s">
+        <v>488</v>
+      </c>
+      <c r="E123" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>494</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>495</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C124" t="s">
         <v>496</v>
       </c>
-      <c r="D123" t="s">
-        <v>492</v>
-      </c>
-      <c r="E123" t="s">
+      <c r="D124" t="s">
+        <v>488</v>
+      </c>
+      <c r="E124" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>498</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B125" t="s">
         <v>499</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C125" t="s">
         <v>500</v>
       </c>
-      <c r="D124" t="s">
-        <v>492</v>
-      </c>
-      <c r="E124" t="s">
+      <c r="D125" t="s">
+        <v>488</v>
+      </c>
+      <c r="E125" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A125" t="s">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>502</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>503</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>504</v>
       </c>
-      <c r="D125" t="s">
-        <v>492</v>
-      </c>
-      <c r="E125" t="s">
+      <c r="D126" t="s">
+        <v>488</v>
+      </c>
+      <c r="E126" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>506</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B127" t="s">
         <v>507</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C127" t="s">
         <v>508</v>
       </c>
-      <c r="D126" t="s">
-        <v>492</v>
-      </c>
-      <c r="E126" t="s">
+      <c r="D127" t="s">
+        <v>488</v>
+      </c>
+      <c r="E127" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>510</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B128" t="s">
         <v>511</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C128" t="s">
         <v>512</v>
       </c>
-      <c r="D127" t="s">
-        <v>492</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="D128" t="s">
+        <v>488</v>
+      </c>
+      <c r="E128" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>514</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>515</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>516</v>
       </c>
-      <c r="D128" t="s">
-        <v>492</v>
-      </c>
-      <c r="E128" t="s">
+      <c r="D129" t="s">
+        <v>488</v>
+      </c>
+      <c r="E129" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>518</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" t="s">
         <v>519</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C130" t="s">
         <v>520</v>
       </c>
-      <c r="D129" t="s">
-        <v>492</v>
-      </c>
-      <c r="E129" t="s">
+      <c r="D130" t="s">
+        <v>488</v>
+      </c>
+      <c r="E130" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>522</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B131" t="s">
         <v>523</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>524</v>
       </c>
-      <c r="D130" t="s">
-        <v>492</v>
-      </c>
-      <c r="E130" t="s">
+      <c r="D131" t="s">
+        <v>488</v>
+      </c>
+      <c r="E131" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>526</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" t="s">
         <v>527</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>528</v>
       </c>
-      <c r="D131" t="s">
-        <v>492</v>
-      </c>
-      <c r="E131" t="s">
+      <c r="D132" t="s">
+        <v>488</v>
+      </c>
+      <c r="E132" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>530</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B133" t="s">
         <v>531</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C133" t="s">
+        <v>691</v>
+      </c>
+      <c r="D133" t="s">
+        <v>488</v>
+      </c>
+      <c r="E133" t="s">
         <v>532</v>
       </c>
-      <c r="D132" t="s">
-        <v>492</v>
-      </c>
-      <c r="E132" t="s">
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+      <c r="B134" t="s">
         <v>534</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C134" t="s">
         <v>535</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D134" t="s">
+        <v>488</v>
+      </c>
+      <c r="E134" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>536</v>
       </c>
-      <c r="D133" t="s">
-        <v>492</v>
-      </c>
-      <c r="E133" t="s">
+      <c r="B135" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+      <c r="C135" t="s">
         <v>538</v>
       </c>
-      <c r="B134" t="s">
+      <c r="D135" t="s">
+        <v>488</v>
+      </c>
+      <c r="E135" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>539</v>
       </c>
-      <c r="C134" t="s">
+      <c r="B136" t="s">
         <v>540</v>
       </c>
-      <c r="D134" t="s">
-        <v>492</v>
-      </c>
-      <c r="E134" t="s">
+      <c r="C136" t="s">
+        <v>520</v>
+      </c>
+      <c r="D136" t="s">
+        <v>488</v>
+      </c>
+      <c r="E136" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>541</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B137" t="s">
         <v>542</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C137" t="s">
         <v>543</v>
       </c>
-      <c r="D135" t="s">
-        <v>492</v>
-      </c>
-      <c r="E135" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A136" t="s">
+      <c r="D137" t="s">
+        <v>488</v>
+      </c>
+      <c r="E137" t="s">
         <v>544</v>
       </c>
-      <c r="B136" t="s">
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>545</v>
       </c>
-      <c r="C136" t="s">
-        <v>524</v>
-      </c>
-      <c r="D136" t="s">
-        <v>492</v>
-      </c>
-      <c r="E136" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
+      <c r="B138" t="s">
         <v>546</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C138" t="s">
         <v>547</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D138" t="s">
+        <v>488</v>
+      </c>
+      <c r="E138" t="s">
         <v>548</v>
       </c>
-      <c r="D137" t="s">
-        <v>492</v>
-      </c>
-      <c r="E137" t="s">
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
+      <c r="B139" t="s">
         <v>550</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C139" t="s">
         <v>551</v>
       </c>
-      <c r="C138" t="s">
+      <c r="D139" t="s">
+        <v>488</v>
+      </c>
+      <c r="E139" t="s">
         <v>552</v>
       </c>
-      <c r="D138" t="s">
-        <v>492</v>
-      </c>
-      <c r="E138" t="s">
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>510</v>
+      </c>
+      <c r="B140" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
+      <c r="C140" t="s">
+        <v>512</v>
+      </c>
+      <c r="D140" t="s">
+        <v>488</v>
+      </c>
+      <c r="E140" t="s">
         <v>554</v>
       </c>
-      <c r="B139" t="s">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>555</v>
       </c>
-      <c r="C139" t="s">
+      <c r="B141" t="s">
         <v>556</v>
       </c>
-      <c r="D139" t="s">
-        <v>492</v>
-      </c>
-      <c r="E139" t="s">
+      <c r="C141" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A140" t="s">
-        <v>514</v>
-      </c>
-      <c r="B140" t="s">
+      <c r="D141" t="s">
+        <v>488</v>
+      </c>
+      <c r="E141" t="s">
         <v>558</v>
       </c>
-      <c r="C140" t="s">
-        <v>516</v>
-      </c>
-      <c r="D140" t="s">
-        <v>492</v>
-      </c>
-      <c r="E140" t="s">
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A141" t="s">
+      <c r="B142" t="s">
         <v>560</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C142" t="s">
         <v>561</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D142" t="s">
+        <v>488</v>
+      </c>
+      <c r="E142" t="s">
         <v>562</v>
       </c>
-      <c r="D141" t="s">
-        <v>492</v>
-      </c>
-      <c r="E141" t="s">
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A142" t="s">
+      <c r="B143" t="s">
         <v>564</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C143" t="s">
+        <v>508</v>
+      </c>
+      <c r="D143" t="s">
+        <v>488</v>
+      </c>
+      <c r="E143" t="s">
         <v>565</v>
       </c>
-      <c r="C142" t="s">
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>566</v>
       </c>
-      <c r="D142" t="s">
-        <v>492</v>
-      </c>
-      <c r="E142" t="s">
+      <c r="B144" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
+      <c r="C144" t="s">
         <v>568</v>
       </c>
-      <c r="B143" t="s">
+      <c r="D144" t="s">
+        <v>488</v>
+      </c>
+      <c r="E144" t="s">
         <v>569</v>
       </c>
-      <c r="C143" t="s">
-        <v>512</v>
-      </c>
-      <c r="D143" t="s">
-        <v>492</v>
-      </c>
-      <c r="E143" t="s">
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+      <c r="B145" t="s">
         <v>571</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C145" t="s">
         <v>572</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D145" t="s">
+        <v>488</v>
+      </c>
+      <c r="E145" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
         <v>573</v>
       </c>
-      <c r="D144" t="s">
-        <v>492</v>
-      </c>
-      <c r="E144" t="s">
+      <c r="B146" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
+      <c r="C146" t="s">
         <v>575</v>
       </c>
-      <c r="B145" t="s">
+      <c r="D146" t="s">
+        <v>488</v>
+      </c>
+      <c r="E146" t="s">
         <v>576</v>
       </c>
-      <c r="C145" t="s">
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
         <v>577</v>
       </c>
-      <c r="D145" t="s">
-        <v>492</v>
-      </c>
-      <c r="E145" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
+      <c r="B147" t="s">
         <v>578</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C147" t="s">
         <v>579</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D147" t="s">
+        <v>488</v>
+      </c>
+      <c r="E147" t="s">
         <v>580</v>
       </c>
-      <c r="D146" t="s">
-        <v>492</v>
-      </c>
-      <c r="E146" t="s">
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
+      <c r="B148" t="s">
         <v>582</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C148" t="s">
+        <v>500</v>
+      </c>
+      <c r="D148" t="s">
+        <v>488</v>
+      </c>
+      <c r="E148" t="s">
         <v>583</v>
       </c>
-      <c r="C147" t="s">
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>584</v>
       </c>
-      <c r="D147" t="s">
-        <v>492</v>
-      </c>
-      <c r="E147" t="s">
+      <c r="B149" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
+      <c r="C149" t="s">
         <v>586</v>
       </c>
-      <c r="B148" t="s">
+      <c r="D149" t="s">
+        <v>488</v>
+      </c>
+      <c r="E149" t="s">
         <v>587</v>
       </c>
-      <c r="C148" t="s">
-        <v>504</v>
-      </c>
-      <c r="D148" t="s">
-        <v>492</v>
-      </c>
-      <c r="E148" t="s">
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
+      <c r="B150" t="s">
         <v>589</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C150" t="s">
         <v>590</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D150" t="s">
+        <v>488</v>
+      </c>
+      <c r="E150" t="s">
         <v>591</v>
       </c>
-      <c r="D149" t="s">
-        <v>492</v>
-      </c>
-      <c r="E149" t="s">
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>536</v>
+      </c>
+      <c r="B151" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
-        <v>593</v>
-      </c>
-      <c r="B150" t="s">
-        <v>594</v>
-      </c>
-      <c r="C150" t="s">
-        <v>595</v>
-      </c>
-      <c r="D150" t="s">
-        <v>492</v>
-      </c>
-      <c r="E150" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A151" t="s">
-        <v>541</v>
-      </c>
-      <c r="B151" t="s">
-        <v>597</v>
-      </c>
       <c r="C151" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="D151" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="E151" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="15.5" x14ac:dyDescent="0.35"/>
+        <v>517</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E151" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E33 A58:E58 A56:B56 D56:E56 A35:E55 A34:B34 D34:E34 A60:E132 A59:B59 D59:E59 A57:B57 D57:E57 A134:E151 A133:B133 D133:E133" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -5083,62 +5082,62 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="B1" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>45607</v>
       </c>
       <c r="B2" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>45618</v>
       </c>
       <c r="B3" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>45638</v>
       </c>
       <c r="B4" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>45651</v>
       </c>
       <c r="B5" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>45670</v>
       </c>
       <c r="B6" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>45702</v>
       </c>
       <c r="B7" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -5155,246 +5154,246 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>601</v>
+      </c>
+      <c r="B1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1" t="s">
+        <v>603</v>
+      </c>
+      <c r="D1" t="s">
+        <v>604</v>
+      </c>
+      <c r="E1" t="s">
+        <v>605</v>
+      </c>
+      <c r="F1" t="s">
         <v>606</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>607</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>608</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>609</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
         <v>610</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E2" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
         <v>612</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>613</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>614</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>615</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D3" t="s">
         <v>616</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>618</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>619</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>620</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>621</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>622</v>
       </c>
-      <c r="F3" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="F4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>623</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>624</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>625</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>626</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>627</v>
       </c>
-      <c r="F4" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="F5" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>628</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>629</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>630</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>631</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>632</v>
       </c>
-      <c r="F5" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>633</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>634</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>635</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>636</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>637</v>
       </c>
-      <c r="F6" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="F7" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>638</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>639</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>640</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>641</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>642</v>
       </c>
-      <c r="F7" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="F8" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>643</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>644</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>645</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>646</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>647</v>
       </c>
-      <c r="F8" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="F9" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>648</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>649</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>650</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>651</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>652</v>
       </c>
-      <c r="F9" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="F10" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>653</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
+        <v>649</v>
+      </c>
+      <c r="C11" t="s">
         <v>654</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
+        <v>651</v>
+      </c>
+      <c r="E11" t="s">
         <v>655</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F11" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>656</v>
       </c>
-      <c r="E10" t="s">
+      <c r="B12" t="s">
         <v>657</v>
       </c>
-      <c r="F10" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
         <v>658</v>
       </c>
-      <c r="B11" t="s">
-        <v>654</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D12" t="s">
         <v>659</v>
       </c>
-      <c r="D11" t="s">
-        <v>656</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>660</v>
       </c>
-      <c r="F11" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>661</v>
-      </c>
-      <c r="B12" t="s">
-        <v>662</v>
-      </c>
-      <c r="C12" t="s">
-        <v>663</v>
-      </c>
-      <c r="D12" t="s">
-        <v>664</v>
-      </c>
-      <c r="E12" t="s">
-        <v>665</v>
-      </c>
       <c r="F12" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -5411,110 +5410,110 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>661</v>
+      </c>
+      <c r="B1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>663</v>
+      </c>
+      <c r="B2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B3" t="s">
         <v>666</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
         <v>668</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
         <v>670</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
         <v>672</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
         <v>674</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
         <v>676</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
         <v>678</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
         <v>680</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B11" t="s">
         <v>682</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B12" t="s">
         <v>684</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B13" t="s">
         <v>686</v>
-      </c>
-      <c r="B11" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>688</v>
-      </c>
-      <c r="B12" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>690</v>
-      </c>
-      <c r="B13" t="s">
-        <v>691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Database and Shaula image
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Javascript\Vers 4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E89B07-FA4B-4EE4-9A61-5C407AEF93B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79030FA-1F56-4D52-BD1F-F67502BF9CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -301,9 +301,6 @@
     <t>  Shaula is a bright star located in the constellation Scorpius. It is one of the brightest stars in the sky and is part of a binary system with a massive companion. Shaula is a blue giant, located about 700 light-years away from Earth, and has a luminosity that is several thousand times greater than the Sun’s. The star is nearing the end of its life and will eventually explode as a supernova. Shaula’s position in the sky, near the "stinger" of the scorpion, has made it a prominent feature in both ancient and modern astronomy.</t>
   </si>
   <si>
-    <t>Images/Shaula.jpg</t>
-  </si>
-  <si>
     <t>Mass: 1.989 x 10^30 kg&lt;br&gt;Distance from Earth: 700 light years&lt;br&gt;Discovered: Known since Ancient Times</t>
   </si>
   <si>
@@ -2117,6 +2114,9 @@
   </si>
   <si>
     <t>Images/XTE_J1550_564.JPG</t>
+  </si>
+  <si>
+    <t>Images/Shaula.webp</t>
   </si>
 </sst>
 </file>
@@ -2495,8 +2495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2883,2195 +2883,2195 @@
         <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>691</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
         <v>94</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>95</v>
-      </c>
-      <c r="C24" t="s">
-        <v>96</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>100</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" t="s">
         <v>102</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>103</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
         <v>106</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>107</v>
-      </c>
-      <c r="C27" t="s">
-        <v>108</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" t="s">
         <v>110</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>111</v>
-      </c>
-      <c r="C28" t="s">
-        <v>112</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
         <v>114</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>115</v>
-      </c>
-      <c r="C29" t="s">
-        <v>116</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" t="s">
         <v>118</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>119</v>
-      </c>
-      <c r="C30" t="s">
-        <v>120</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
         <v>122</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>123</v>
-      </c>
-      <c r="C31" t="s">
-        <v>124</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" t="s">
         <v>126</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>127</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>128</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>129</v>
-      </c>
-      <c r="E32" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" t="s">
         <v>131</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>132</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" t="s">
         <v>133</v>
-      </c>
-      <c r="D33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E33" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" t="s">
         <v>135</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>687</v>
+      </c>
+      <c r="D34" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" t="s">
         <v>136</v>
-      </c>
-      <c r="C34" t="s">
-        <v>688</v>
-      </c>
-      <c r="D34" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" t="s">
         <v>138</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>139</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" t="s">
         <v>140</v>
-      </c>
-      <c r="D35" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" t="s">
         <v>142</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>143</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" t="s">
         <v>144</v>
-      </c>
-      <c r="D36" t="s">
-        <v>129</v>
-      </c>
-      <c r="E36" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
+        <v>145</v>
+      </c>
+      <c r="B37" t="s">
         <v>146</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>147</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>128</v>
+      </c>
+      <c r="E37" t="s">
         <v>148</v>
-      </c>
-      <c r="D37" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" t="s">
         <v>150</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>151</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" t="s">
         <v>152</v>
-      </c>
-      <c r="D38" t="s">
-        <v>129</v>
-      </c>
-      <c r="E38" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
         <v>154</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>155</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" t="s">
         <v>156</v>
-      </c>
-      <c r="D39" t="s">
-        <v>129</v>
-      </c>
-      <c r="E39" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" t="s">
         <v>158</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>159</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" t="s">
         <v>160</v>
-      </c>
-      <c r="D40" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B41" t="s">
         <v>162</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>163</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" t="s">
         <v>164</v>
-      </c>
-      <c r="D41" t="s">
-        <v>129</v>
-      </c>
-      <c r="E41" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" t="s">
         <v>166</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>167</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" t="s">
         <v>168</v>
-      </c>
-      <c r="D42" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" t="s">
         <v>170</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>171</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" t="s">
         <v>172</v>
-      </c>
-      <c r="D43" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" t="s">
         <v>174</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>175</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" t="s">
         <v>176</v>
-      </c>
-      <c r="D44" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" t="s">
         <v>178</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>179</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" t="s">
         <v>180</v>
-      </c>
-      <c r="D45" t="s">
-        <v>129</v>
-      </c>
-      <c r="E45" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" t="s">
         <v>182</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>183</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" t="s">
         <v>184</v>
-      </c>
-      <c r="D46" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" t="s">
         <v>186</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>187</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" t="s">
         <v>188</v>
-      </c>
-      <c r="D47" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>189</v>
+      </c>
+      <c r="B48" t="s">
         <v>190</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>191</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" t="s">
         <v>192</v>
-      </c>
-      <c r="D48" t="s">
-        <v>129</v>
-      </c>
-      <c r="E48" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" t="s">
         <v>194</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>195</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" t="s">
         <v>196</v>
-      </c>
-      <c r="D49" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>197</v>
+      </c>
+      <c r="B50" t="s">
         <v>198</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>199</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" t="s">
         <v>200</v>
-      </c>
-      <c r="D50" t="s">
-        <v>129</v>
-      </c>
-      <c r="E50" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" t="s">
         <v>202</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>203</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" t="s">
         <v>204</v>
-      </c>
-      <c r="D51" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" t="s">
         <v>206</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>207</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" t="s">
         <v>208</v>
-      </c>
-      <c r="D52" t="s">
-        <v>129</v>
-      </c>
-      <c r="E52" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
+        <v>209</v>
+      </c>
+      <c r="B53" t="s">
         <v>210</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>211</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" t="s">
         <v>212</v>
-      </c>
-      <c r="D53" t="s">
-        <v>129</v>
-      </c>
-      <c r="E53" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" t="s">
         <v>214</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>215</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>128</v>
+      </c>
+      <c r="E54" t="s">
         <v>216</v>
-      </c>
-      <c r="D54" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
+        <v>217</v>
+      </c>
+      <c r="B55" t="s">
         <v>218</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>219</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" t="s">
         <v>220</v>
-      </c>
-      <c r="D55" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>221</v>
+      </c>
+      <c r="B56" t="s">
         <v>222</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>686</v>
+      </c>
+      <c r="D56" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" t="s">
         <v>223</v>
-      </c>
-      <c r="C56" t="s">
-        <v>687</v>
-      </c>
-      <c r="D56" t="s">
-        <v>129</v>
-      </c>
-      <c r="E56" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
+        <v>224</v>
+      </c>
+      <c r="B57" t="s">
         <v>225</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>689</v>
+      </c>
+      <c r="D57" t="s">
+        <v>128</v>
+      </c>
+      <c r="E57" t="s">
         <v>226</v>
-      </c>
-      <c r="C57" t="s">
-        <v>690</v>
-      </c>
-      <c r="D57" t="s">
-        <v>129</v>
-      </c>
-      <c r="E57" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
+        <v>227</v>
+      </c>
+      <c r="B58" t="s">
         <v>228</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>229</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
+        <v>128</v>
+      </c>
+      <c r="E58" t="s">
         <v>230</v>
-      </c>
-      <c r="D58" t="s">
-        <v>129</v>
-      </c>
-      <c r="E58" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59" t="s">
         <v>232</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>688</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+      <c r="E59" t="s">
         <v>233</v>
-      </c>
-      <c r="C59" t="s">
-        <v>689</v>
-      </c>
-      <c r="D59" t="s">
-        <v>129</v>
-      </c>
-      <c r="E59" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
+        <v>234</v>
+      </c>
+      <c r="B60" t="s">
         <v>235</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>236</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
+        <v>128</v>
+      </c>
+      <c r="E60" t="s">
         <v>237</v>
-      </c>
-      <c r="D60" t="s">
-        <v>129</v>
-      </c>
-      <c r="E60" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
+        <v>238</v>
+      </c>
+      <c r="B61" t="s">
         <v>239</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>240</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
+        <v>128</v>
+      </c>
+      <c r="E61" t="s">
         <v>241</v>
-      </c>
-      <c r="D61" t="s">
-        <v>129</v>
-      </c>
-      <c r="E61" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>242</v>
+      </c>
+      <c r="B62" t="s">
         <v>243</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>244</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>245</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>246</v>
-      </c>
-      <c r="E62" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
+        <v>247</v>
+      </c>
+      <c r="B63" t="s">
         <v>248</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>249</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
+        <v>245</v>
+      </c>
+      <c r="E63" t="s">
         <v>250</v>
-      </c>
-      <c r="D63" t="s">
-        <v>246</v>
-      </c>
-      <c r="E63" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
+        <v>251</v>
+      </c>
+      <c r="B64" t="s">
         <v>252</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>253</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
+        <v>245</v>
+      </c>
+      <c r="E64" t="s">
         <v>254</v>
-      </c>
-      <c r="D64" t="s">
-        <v>246</v>
-      </c>
-      <c r="E64" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
+        <v>255</v>
+      </c>
+      <c r="B65" t="s">
         <v>256</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>257</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
+        <v>245</v>
+      </c>
+      <c r="E65" t="s">
         <v>258</v>
-      </c>
-      <c r="D65" t="s">
-        <v>246</v>
-      </c>
-      <c r="E65" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>259</v>
+      </c>
+      <c r="B66" t="s">
         <v>260</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>261</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
+        <v>245</v>
+      </c>
+      <c r="E66" t="s">
         <v>262</v>
-      </c>
-      <c r="D66" t="s">
-        <v>246</v>
-      </c>
-      <c r="E66" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" t="s">
         <v>264</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>265</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
+        <v>245</v>
+      </c>
+      <c r="E67" t="s">
         <v>266</v>
-      </c>
-      <c r="D67" t="s">
-        <v>246</v>
-      </c>
-      <c r="E67" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>267</v>
+      </c>
+      <c r="B68" t="s">
         <v>268</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>269</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
+        <v>245</v>
+      </c>
+      <c r="E68" t="s">
         <v>270</v>
-      </c>
-      <c r="D68" t="s">
-        <v>246</v>
-      </c>
-      <c r="E68" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
+        <v>271</v>
+      </c>
+      <c r="B69" t="s">
         <v>272</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>273</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>245</v>
+      </c>
+      <c r="E69" t="s">
         <v>274</v>
-      </c>
-      <c r="D69" t="s">
-        <v>246</v>
-      </c>
-      <c r="E69" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>275</v>
+      </c>
+      <c r="B70" t="s">
         <v>276</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>277</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
+        <v>245</v>
+      </c>
+      <c r="E70" t="s">
         <v>278</v>
-      </c>
-      <c r="D70" t="s">
-        <v>246</v>
-      </c>
-      <c r="E70" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>279</v>
+      </c>
+      <c r="B71" t="s">
         <v>280</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>281</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
+        <v>245</v>
+      </c>
+      <c r="E71" t="s">
         <v>282</v>
-      </c>
-      <c r="D71" t="s">
-        <v>246</v>
-      </c>
-      <c r="E71" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>283</v>
+      </c>
+      <c r="B72" t="s">
         <v>284</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>285</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
+        <v>245</v>
+      </c>
+      <c r="E72" t="s">
         <v>286</v>
-      </c>
-      <c r="D72" t="s">
-        <v>246</v>
-      </c>
-      <c r="E72" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
+        <v>287</v>
+      </c>
+      <c r="B73" t="s">
         <v>288</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>289</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
+        <v>245</v>
+      </c>
+      <c r="E73" t="s">
         <v>290</v>
-      </c>
-      <c r="D73" t="s">
-        <v>246</v>
-      </c>
-      <c r="E73" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" t="s">
         <v>292</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>293</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
+        <v>245</v>
+      </c>
+      <c r="E74" t="s">
         <v>294</v>
-      </c>
-      <c r="D74" t="s">
-        <v>246</v>
-      </c>
-      <c r="E74" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
+        <v>295</v>
+      </c>
+      <c r="B75" t="s">
         <v>296</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>297</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
+        <v>245</v>
+      </c>
+      <c r="E75" t="s">
         <v>298</v>
-      </c>
-      <c r="D75" t="s">
-        <v>246</v>
-      </c>
-      <c r="E75" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
+        <v>299</v>
+      </c>
+      <c r="B76" t="s">
         <v>300</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>301</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
+        <v>245</v>
+      </c>
+      <c r="E76" t="s">
         <v>302</v>
-      </c>
-      <c r="D76" t="s">
-        <v>246</v>
-      </c>
-      <c r="E76" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>303</v>
+      </c>
+      <c r="B77" t="s">
         <v>304</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>305</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
+        <v>245</v>
+      </c>
+      <c r="E77" t="s">
         <v>306</v>
-      </c>
-      <c r="D77" t="s">
-        <v>246</v>
-      </c>
-      <c r="E77" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
+        <v>307</v>
+      </c>
+      <c r="B78" t="s">
         <v>308</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>309</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
+        <v>245</v>
+      </c>
+      <c r="E78" t="s">
         <v>310</v>
-      </c>
-      <c r="D78" t="s">
-        <v>246</v>
-      </c>
-      <c r="E78" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
+        <v>311</v>
+      </c>
+      <c r="B79" t="s">
         <v>312</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>313</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>245</v>
+      </c>
+      <c r="E79" t="s">
         <v>314</v>
-      </c>
-      <c r="D79" t="s">
-        <v>246</v>
-      </c>
-      <c r="E79" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
+        <v>315</v>
+      </c>
+      <c r="B80" t="s">
         <v>316</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>317</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
+        <v>245</v>
+      </c>
+      <c r="E80" t="s">
         <v>318</v>
-      </c>
-      <c r="D80" t="s">
-        <v>246</v>
-      </c>
-      <c r="E80" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
+        <v>319</v>
+      </c>
+      <c r="B81" t="s">
         <v>320</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>321</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
+        <v>245</v>
+      </c>
+      <c r="E81" t="s">
         <v>322</v>
-      </c>
-      <c r="D81" t="s">
-        <v>246</v>
-      </c>
-      <c r="E81" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>323</v>
+      </c>
+      <c r="B82" t="s">
         <v>324</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>325</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
+        <v>245</v>
+      </c>
+      <c r="E82" t="s">
         <v>326</v>
-      </c>
-      <c r="D82" t="s">
-        <v>246</v>
-      </c>
-      <c r="E82" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
+        <v>327</v>
+      </c>
+      <c r="B83" t="s">
         <v>328</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>329</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
+        <v>245</v>
+      </c>
+      <c r="E83" t="s">
         <v>330</v>
-      </c>
-      <c r="D83" t="s">
-        <v>246</v>
-      </c>
-      <c r="E83" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
+        <v>331</v>
+      </c>
+      <c r="B84" t="s">
         <v>332</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>333</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
+        <v>245</v>
+      </c>
+      <c r="E84" t="s">
         <v>334</v>
-      </c>
-      <c r="D84" t="s">
-        <v>246</v>
-      </c>
-      <c r="E84" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
+        <v>335</v>
+      </c>
+      <c r="B85" t="s">
         <v>336</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>337</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>245</v>
+      </c>
+      <c r="E85" t="s">
         <v>338</v>
-      </c>
-      <c r="D85" t="s">
-        <v>246</v>
-      </c>
-      <c r="E85" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
+        <v>339</v>
+      </c>
+      <c r="B86" t="s">
         <v>340</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>341</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>245</v>
+      </c>
+      <c r="E86" t="s">
         <v>342</v>
-      </c>
-      <c r="D86" t="s">
-        <v>246</v>
-      </c>
-      <c r="E86" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
+        <v>343</v>
+      </c>
+      <c r="B87" t="s">
         <v>344</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>345</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
+        <v>245</v>
+      </c>
+      <c r="E87" t="s">
         <v>346</v>
-      </c>
-      <c r="D87" t="s">
-        <v>246</v>
-      </c>
-      <c r="E87" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
+        <v>347</v>
+      </c>
+      <c r="B88" t="s">
         <v>348</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>349</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
+        <v>245</v>
+      </c>
+      <c r="E88" t="s">
         <v>350</v>
-      </c>
-      <c r="D88" t="s">
-        <v>246</v>
-      </c>
-      <c r="E88" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
+        <v>351</v>
+      </c>
+      <c r="B89" t="s">
         <v>352</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>353</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
+        <v>245</v>
+      </c>
+      <c r="E89" t="s">
         <v>354</v>
-      </c>
-      <c r="D89" t="s">
-        <v>246</v>
-      </c>
-      <c r="E89" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
+        <v>355</v>
+      </c>
+      <c r="B90" t="s">
         <v>356</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>357</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
+        <v>245</v>
+      </c>
+      <c r="E90" t="s">
         <v>358</v>
-      </c>
-      <c r="D90" t="s">
-        <v>246</v>
-      </c>
-      <c r="E90" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
+        <v>359</v>
+      </c>
+      <c r="B91" t="s">
         <v>360</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>361</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
+        <v>245</v>
+      </c>
+      <c r="E91" t="s">
         <v>362</v>
-      </c>
-      <c r="D91" t="s">
-        <v>246</v>
-      </c>
-      <c r="E91" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
+        <v>363</v>
+      </c>
+      <c r="B92" t="s">
         <v>364</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>365</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>366</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>367</v>
-      </c>
-      <c r="E92" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
+        <v>368</v>
+      </c>
+      <c r="B93" t="s">
         <v>369</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>370</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
+        <v>366</v>
+      </c>
+      <c r="E93" t="s">
         <v>371</v>
-      </c>
-      <c r="D93" t="s">
-        <v>367</v>
-      </c>
-      <c r="E93" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
+        <v>372</v>
+      </c>
+      <c r="B94" t="s">
         <v>373</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>374</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
+        <v>366</v>
+      </c>
+      <c r="E94" t="s">
         <v>375</v>
-      </c>
-      <c r="D94" t="s">
-        <v>367</v>
-      </c>
-      <c r="E94" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
+        <v>376</v>
+      </c>
+      <c r="B95" t="s">
         <v>377</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>378</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
+        <v>366</v>
+      </c>
+      <c r="E95" t="s">
         <v>379</v>
-      </c>
-      <c r="D95" t="s">
-        <v>367</v>
-      </c>
-      <c r="E95" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
+        <v>380</v>
+      </c>
+      <c r="B96" t="s">
         <v>381</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>382</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
+        <v>366</v>
+      </c>
+      <c r="E96" t="s">
         <v>383</v>
-      </c>
-      <c r="D96" t="s">
-        <v>367</v>
-      </c>
-      <c r="E96" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
+        <v>384</v>
+      </c>
+      <c r="B97" t="s">
         <v>385</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>386</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
+        <v>366</v>
+      </c>
+      <c r="E97" t="s">
         <v>387</v>
-      </c>
-      <c r="D97" t="s">
-        <v>367</v>
-      </c>
-      <c r="E97" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
+        <v>388</v>
+      </c>
+      <c r="B98" t="s">
         <v>389</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>390</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
+        <v>366</v>
+      </c>
+      <c r="E98" t="s">
         <v>391</v>
-      </c>
-      <c r="D98" t="s">
-        <v>367</v>
-      </c>
-      <c r="E98" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
+        <v>392</v>
+      </c>
+      <c r="B99" t="s">
         <v>393</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>394</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
+        <v>366</v>
+      </c>
+      <c r="E99" t="s">
         <v>395</v>
-      </c>
-      <c r="D99" t="s">
-        <v>367</v>
-      </c>
-      <c r="E99" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
+        <v>396</v>
+      </c>
+      <c r="B100" t="s">
         <v>397</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>398</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
+        <v>366</v>
+      </c>
+      <c r="E100" t="s">
         <v>399</v>
-      </c>
-      <c r="D100" t="s">
-        <v>367</v>
-      </c>
-      <c r="E100" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>400</v>
+      </c>
+      <c r="B101" t="s">
         <v>401</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>402</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
+        <v>366</v>
+      </c>
+      <c r="E101" t="s">
         <v>403</v>
-      </c>
-      <c r="D101" t="s">
-        <v>367</v>
-      </c>
-      <c r="E101" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
+        <v>404</v>
+      </c>
+      <c r="B102" t="s">
         <v>405</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>406</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
+        <v>366</v>
+      </c>
+      <c r="E102" t="s">
         <v>407</v>
-      </c>
-      <c r="D102" t="s">
-        <v>367</v>
-      </c>
-      <c r="E102" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
+        <v>408</v>
+      </c>
+      <c r="B103" t="s">
         <v>409</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>410</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
+        <v>366</v>
+      </c>
+      <c r="E103" t="s">
         <v>411</v>
-      </c>
-      <c r="D103" t="s">
-        <v>367</v>
-      </c>
-      <c r="E103" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
+        <v>412</v>
+      </c>
+      <c r="B104" t="s">
         <v>413</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>414</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
+        <v>366</v>
+      </c>
+      <c r="E104" t="s">
         <v>415</v>
-      </c>
-      <c r="D104" t="s">
-        <v>367</v>
-      </c>
-      <c r="E104" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
+        <v>416</v>
+      </c>
+      <c r="B105" t="s">
         <v>417</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>418</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
+        <v>366</v>
+      </c>
+      <c r="E105" t="s">
         <v>419</v>
-      </c>
-      <c r="D105" t="s">
-        <v>367</v>
-      </c>
-      <c r="E105" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
+        <v>420</v>
+      </c>
+      <c r="B106" t="s">
         <v>421</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>422</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>366</v>
+      </c>
+      <c r="E106" t="s">
         <v>423</v>
-      </c>
-      <c r="D106" t="s">
-        <v>367</v>
-      </c>
-      <c r="E106" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>424</v>
+      </c>
+      <c r="B107" t="s">
         <v>425</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>426</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
+        <v>366</v>
+      </c>
+      <c r="E107" t="s">
         <v>427</v>
-      </c>
-      <c r="D107" t="s">
-        <v>367</v>
-      </c>
-      <c r="E107" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
+        <v>428</v>
+      </c>
+      <c r="B108" t="s">
         <v>429</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>430</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>366</v>
+      </c>
+      <c r="E108" t="s">
         <v>431</v>
-      </c>
-      <c r="D108" t="s">
-        <v>367</v>
-      </c>
-      <c r="E108" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
+        <v>432</v>
+      </c>
+      <c r="B109" t="s">
         <v>433</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>434</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
+        <v>366</v>
+      </c>
+      <c r="E109" t="s">
         <v>435</v>
-      </c>
-      <c r="D109" t="s">
-        <v>367</v>
-      </c>
-      <c r="E109" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
+        <v>436</v>
+      </c>
+      <c r="B110" t="s">
         <v>437</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>438</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
+        <v>366</v>
+      </c>
+      <c r="E110" t="s">
         <v>439</v>
-      </c>
-      <c r="D110" t="s">
-        <v>367</v>
-      </c>
-      <c r="E110" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
+        <v>440</v>
+      </c>
+      <c r="B111" t="s">
         <v>441</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>442</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
+        <v>366</v>
+      </c>
+      <c r="E111" t="s">
         <v>443</v>
-      </c>
-      <c r="D111" t="s">
-        <v>367</v>
-      </c>
-      <c r="E111" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
+        <v>444</v>
+      </c>
+      <c r="B112" t="s">
         <v>445</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>446</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
+        <v>366</v>
+      </c>
+      <c r="E112" t="s">
         <v>447</v>
-      </c>
-      <c r="D112" t="s">
-        <v>367</v>
-      </c>
-      <c r="E112" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
+        <v>448</v>
+      </c>
+      <c r="B113" t="s">
         <v>449</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>450</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
+        <v>366</v>
+      </c>
+      <c r="E113" t="s">
         <v>451</v>
-      </c>
-      <c r="D113" t="s">
-        <v>367</v>
-      </c>
-      <c r="E113" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
+        <v>452</v>
+      </c>
+      <c r="B114" t="s">
         <v>453</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>454</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
+        <v>366</v>
+      </c>
+      <c r="E114" t="s">
         <v>455</v>
-      </c>
-      <c r="D114" t="s">
-        <v>367</v>
-      </c>
-      <c r="E114" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
+        <v>456</v>
+      </c>
+      <c r="B115" t="s">
         <v>457</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>458</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
+        <v>366</v>
+      </c>
+      <c r="E115" t="s">
         <v>459</v>
-      </c>
-      <c r="D115" t="s">
-        <v>367</v>
-      </c>
-      <c r="E115" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
+        <v>460</v>
+      </c>
+      <c r="B116" t="s">
         <v>461</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>462</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
+        <v>366</v>
+      </c>
+      <c r="E116" t="s">
         <v>463</v>
-      </c>
-      <c r="D116" t="s">
-        <v>367</v>
-      </c>
-      <c r="E116" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
+        <v>464</v>
+      </c>
+      <c r="B117" t="s">
         <v>465</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>466</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
+        <v>366</v>
+      </c>
+      <c r="E117" t="s">
         <v>467</v>
-      </c>
-      <c r="D117" t="s">
-        <v>367</v>
-      </c>
-      <c r="E117" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>468</v>
+      </c>
+      <c r="B118" t="s">
         <v>469</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>470</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
+        <v>366</v>
+      </c>
+      <c r="E118" t="s">
         <v>471</v>
-      </c>
-      <c r="D118" t="s">
-        <v>367</v>
-      </c>
-      <c r="E118" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
+        <v>472</v>
+      </c>
+      <c r="B119" t="s">
         <v>473</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>474</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
+        <v>366</v>
+      </c>
+      <c r="E119" t="s">
         <v>475</v>
-      </c>
-      <c r="D119" t="s">
-        <v>367</v>
-      </c>
-      <c r="E119" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
+        <v>476</v>
+      </c>
+      <c r="B120" t="s">
         <v>477</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>478</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
+        <v>366</v>
+      </c>
+      <c r="E120" t="s">
         <v>479</v>
-      </c>
-      <c r="D120" t="s">
-        <v>367</v>
-      </c>
-      <c r="E120" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
+        <v>480</v>
+      </c>
+      <c r="B121" t="s">
         <v>481</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>482</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
+        <v>366</v>
+      </c>
+      <c r="E121" t="s">
         <v>483</v>
-      </c>
-      <c r="D121" t="s">
-        <v>367</v>
-      </c>
-      <c r="E121" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>484</v>
+      </c>
+      <c r="B122" t="s">
         <v>485</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>486</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
         <v>487</v>
       </c>
-      <c r="D122" t="s">
+      <c r="E122" t="s">
         <v>488</v>
-      </c>
-      <c r="E122" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
+        <v>489</v>
+      </c>
+      <c r="B123" t="s">
         <v>490</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>491</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
+        <v>487</v>
+      </c>
+      <c r="E123" t="s">
         <v>492</v>
-      </c>
-      <c r="D123" t="s">
-        <v>488</v>
-      </c>
-      <c r="E123" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
+        <v>493</v>
+      </c>
+      <c r="B124" t="s">
         <v>494</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>495</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
+        <v>487</v>
+      </c>
+      <c r="E124" t="s">
         <v>496</v>
-      </c>
-      <c r="D124" t="s">
-        <v>488</v>
-      </c>
-      <c r="E124" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
+        <v>497</v>
+      </c>
+      <c r="B125" t="s">
         <v>498</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>499</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D125" t="s">
+        <v>487</v>
+      </c>
+      <c r="E125" t="s">
         <v>500</v>
-      </c>
-      <c r="D125" t="s">
-        <v>488</v>
-      </c>
-      <c r="E125" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
+        <v>501</v>
+      </c>
+      <c r="B126" t="s">
         <v>502</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>503</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
+        <v>487</v>
+      </c>
+      <c r="E126" t="s">
         <v>504</v>
-      </c>
-      <c r="D126" t="s">
-        <v>488</v>
-      </c>
-      <c r="E126" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
+        <v>505</v>
+      </c>
+      <c r="B127" t="s">
         <v>506</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>507</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
+        <v>487</v>
+      </c>
+      <c r="E127" t="s">
         <v>508</v>
-      </c>
-      <c r="D127" t="s">
-        <v>488</v>
-      </c>
-      <c r="E127" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
+        <v>509</v>
+      </c>
+      <c r="B128" t="s">
         <v>510</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>511</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
+        <v>487</v>
+      </c>
+      <c r="E128" t="s">
         <v>512</v>
-      </c>
-      <c r="D128" t="s">
-        <v>488</v>
-      </c>
-      <c r="E128" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
+        <v>513</v>
+      </c>
+      <c r="B129" t="s">
         <v>514</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>515</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
+        <v>487</v>
+      </c>
+      <c r="E129" t="s">
         <v>516</v>
-      </c>
-      <c r="D129" t="s">
-        <v>488</v>
-      </c>
-      <c r="E129" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
+        <v>517</v>
+      </c>
+      <c r="B130" t="s">
         <v>518</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>519</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
+        <v>487</v>
+      </c>
+      <c r="E130" t="s">
         <v>520</v>
-      </c>
-      <c r="D130" t="s">
-        <v>488</v>
-      </c>
-      <c r="E130" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
+        <v>521</v>
+      </c>
+      <c r="B131" t="s">
         <v>522</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>523</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
+        <v>487</v>
+      </c>
+      <c r="E131" t="s">
         <v>524</v>
-      </c>
-      <c r="D131" t="s">
-        <v>488</v>
-      </c>
-      <c r="E131" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
+        <v>525</v>
+      </c>
+      <c r="B132" t="s">
         <v>526</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>527</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
+        <v>487</v>
+      </c>
+      <c r="E132" t="s">
         <v>528</v>
-      </c>
-      <c r="D132" t="s">
-        <v>488</v>
-      </c>
-      <c r="E132" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
+        <v>529</v>
+      </c>
+      <c r="B133" t="s">
         <v>530</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
+        <v>690</v>
+      </c>
+      <c r="D133" t="s">
+        <v>487</v>
+      </c>
+      <c r="E133" t="s">
         <v>531</v>
-      </c>
-      <c r="C133" t="s">
-        <v>691</v>
-      </c>
-      <c r="D133" t="s">
-        <v>488</v>
-      </c>
-      <c r="E133" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
+        <v>532</v>
+      </c>
+      <c r="B134" t="s">
         <v>533</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>534</v>
       </c>
-      <c r="C134" t="s">
-        <v>535</v>
-      </c>
       <c r="D134" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E134" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
+        <v>535</v>
+      </c>
+      <c r="B135" t="s">
         <v>536</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>537</v>
       </c>
-      <c r="C135" t="s">
-        <v>538</v>
-      </c>
       <c r="D135" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E135" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
+        <v>538</v>
+      </c>
+      <c r="B136" t="s">
         <v>539</v>
       </c>
-      <c r="B136" t="s">
-        <v>540</v>
-      </c>
       <c r="C136" t="s">
+        <v>519</v>
+      </c>
+      <c r="D136" t="s">
+        <v>487</v>
+      </c>
+      <c r="E136" t="s">
         <v>520</v>
-      </c>
-      <c r="D136" t="s">
-        <v>488</v>
-      </c>
-      <c r="E136" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
+        <v>540</v>
+      </c>
+      <c r="B137" t="s">
         <v>541</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>542</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
+        <v>487</v>
+      </c>
+      <c r="E137" t="s">
         <v>543</v>
-      </c>
-      <c r="D137" t="s">
-        <v>488</v>
-      </c>
-      <c r="E137" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
+        <v>544</v>
+      </c>
+      <c r="B138" t="s">
         <v>545</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>546</v>
       </c>
-      <c r="C138" t="s">
+      <c r="D138" t="s">
+        <v>487</v>
+      </c>
+      <c r="E138" t="s">
         <v>547</v>
-      </c>
-      <c r="D138" t="s">
-        <v>488</v>
-      </c>
-      <c r="E138" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
+        <v>548</v>
+      </c>
+      <c r="B139" t="s">
         <v>549</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>550</v>
       </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
+        <v>487</v>
+      </c>
+      <c r="E139" t="s">
         <v>551</v>
-      </c>
-      <c r="D139" t="s">
-        <v>488</v>
-      </c>
-      <c r="E139" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B140" t="s">
+        <v>552</v>
+      </c>
+      <c r="C140" t="s">
+        <v>511</v>
+      </c>
+      <c r="D140" t="s">
+        <v>487</v>
+      </c>
+      <c r="E140" t="s">
         <v>553</v>
-      </c>
-      <c r="C140" t="s">
-        <v>512</v>
-      </c>
-      <c r="D140" t="s">
-        <v>488</v>
-      </c>
-      <c r="E140" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
+        <v>554</v>
+      </c>
+      <c r="B141" t="s">
         <v>555</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" t="s">
         <v>556</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
+        <v>487</v>
+      </c>
+      <c r="E141" t="s">
         <v>557</v>
-      </c>
-      <c r="D141" t="s">
-        <v>488</v>
-      </c>
-      <c r="E141" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
+        <v>558</v>
+      </c>
+      <c r="B142" t="s">
         <v>559</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>560</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
+        <v>487</v>
+      </c>
+      <c r="E142" t="s">
         <v>561</v>
-      </c>
-      <c r="D142" t="s">
-        <v>488</v>
-      </c>
-      <c r="E142" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
+        <v>562</v>
+      </c>
+      <c r="B143" t="s">
         <v>563</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
+        <v>507</v>
+      </c>
+      <c r="D143" t="s">
+        <v>487</v>
+      </c>
+      <c r="E143" t="s">
         <v>564</v>
-      </c>
-      <c r="C143" t="s">
-        <v>508</v>
-      </c>
-      <c r="D143" t="s">
-        <v>488</v>
-      </c>
-      <c r="E143" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
+        <v>565</v>
+      </c>
+      <c r="B144" t="s">
         <v>566</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>567</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
+        <v>487</v>
+      </c>
+      <c r="E144" t="s">
         <v>568</v>
-      </c>
-      <c r="D144" t="s">
-        <v>488</v>
-      </c>
-      <c r="E144" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
+        <v>569</v>
+      </c>
+      <c r="B145" t="s">
         <v>570</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
         <v>571</v>
       </c>
-      <c r="C145" t="s">
-        <v>572</v>
-      </c>
       <c r="D145" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E145" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
+        <v>572</v>
+      </c>
+      <c r="B146" t="s">
         <v>573</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" t="s">
         <v>574</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
+        <v>487</v>
+      </c>
+      <c r="E146" t="s">
         <v>575</v>
-      </c>
-      <c r="D146" t="s">
-        <v>488</v>
-      </c>
-      <c r="E146" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
+        <v>576</v>
+      </c>
+      <c r="B147" t="s">
         <v>577</v>
       </c>
-      <c r="B147" t="s">
+      <c r="C147" t="s">
         <v>578</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D147" t="s">
+        <v>487</v>
+      </c>
+      <c r="E147" t="s">
         <v>579</v>
-      </c>
-      <c r="D147" t="s">
-        <v>488</v>
-      </c>
-      <c r="E147" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
+        <v>580</v>
+      </c>
+      <c r="B148" t="s">
         <v>581</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
+        <v>499</v>
+      </c>
+      <c r="D148" t="s">
+        <v>487</v>
+      </c>
+      <c r="E148" t="s">
         <v>582</v>
-      </c>
-      <c r="C148" t="s">
-        <v>500</v>
-      </c>
-      <c r="D148" t="s">
-        <v>488</v>
-      </c>
-      <c r="E148" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
+        <v>583</v>
+      </c>
+      <c r="B149" t="s">
         <v>584</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
         <v>585</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
+        <v>487</v>
+      </c>
+      <c r="E149" t="s">
         <v>586</v>
-      </c>
-      <c r="D149" t="s">
-        <v>488</v>
-      </c>
-      <c r="E149" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
+        <v>587</v>
+      </c>
+      <c r="B150" t="s">
         <v>588</v>
       </c>
-      <c r="B150" t="s">
+      <c r="C150" t="s">
         <v>589</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
+        <v>487</v>
+      </c>
+      <c r="E150" t="s">
         <v>590</v>
-      </c>
-      <c r="D150" t="s">
-        <v>488</v>
-      </c>
-      <c r="E150" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B151" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C151" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D151" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E151" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E33 A58:E58 A56:B56 D56:E56 A35:E55 A34:B34 D34:E34 A60:E132 A59:B59 D59:E59 A57:B57 D57:E57 A134:E151 A133:B133 D133:E133" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:E22 A58:E58 A56:B56 D56:E56 A35:E55 A34:B34 D34:E34 A60:E132 A59:B59 D59:E59 A57:B57 D57:E57 A134:E151 A133:B133 D133:E133 A24:E33 A23:B23 D23:E23" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -5086,10 +5086,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B1" t="s">
         <v>593</v>
-      </c>
-      <c r="B1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -5097,7 +5097,7 @@
         <v>45607</v>
       </c>
       <c r="B2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -5105,7 +5105,7 @@
         <v>45618</v>
       </c>
       <c r="B3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -5113,7 +5113,7 @@
         <v>45638</v>
       </c>
       <c r="B4" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -5121,7 +5121,7 @@
         <v>45651</v>
       </c>
       <c r="B5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -5129,7 +5129,7 @@
         <v>45670</v>
       </c>
       <c r="B6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -5137,7 +5137,7 @@
         <v>45702</v>
       </c>
       <c r="B7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>
@@ -5158,242 +5158,242 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B1" t="s">
         <v>601</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>602</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>603</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>604</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>605</v>
-      </c>
-      <c r="F1" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>606</v>
+      </c>
+      <c r="B2" t="s">
         <v>607</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>608</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>609</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>610</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>611</v>
-      </c>
-      <c r="F2" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B3" t="s">
         <v>613</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>614</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>615</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>616</v>
       </c>
-      <c r="E3" t="s">
-        <v>617</v>
-      </c>
       <c r="F3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>617</v>
+      </c>
+      <c r="B4" t="s">
         <v>618</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>619</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>620</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>621</v>
       </c>
-      <c r="E4" t="s">
-        <v>622</v>
-      </c>
       <c r="F4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>622</v>
+      </c>
+      <c r="B5" t="s">
         <v>623</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>624</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>625</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>626</v>
       </c>
-      <c r="E5" t="s">
-        <v>627</v>
-      </c>
       <c r="F5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>627</v>
+      </c>
+      <c r="B6" t="s">
         <v>628</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>629</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>630</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>631</v>
       </c>
-      <c r="E6" t="s">
-        <v>632</v>
-      </c>
       <c r="F6" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>632</v>
+      </c>
+      <c r="B7" t="s">
         <v>633</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>634</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>635</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>636</v>
       </c>
-      <c r="E7" t="s">
-        <v>637</v>
-      </c>
       <c r="F7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>637</v>
+      </c>
+      <c r="B8" t="s">
         <v>638</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>639</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>640</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>641</v>
       </c>
-      <c r="E8" t="s">
-        <v>642</v>
-      </c>
       <c r="F8" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>642</v>
+      </c>
+      <c r="B9" t="s">
         <v>643</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>644</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>645</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>646</v>
       </c>
-      <c r="E9" t="s">
-        <v>647</v>
-      </c>
       <c r="F9" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" t="s">
         <v>648</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>649</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>650</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>651</v>
       </c>
-      <c r="E10" t="s">
-        <v>652</v>
-      </c>
       <c r="F10" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>652</v>
+      </c>
+      <c r="B11" t="s">
+        <v>648</v>
+      </c>
+      <c r="C11" t="s">
         <v>653</v>
       </c>
-      <c r="B11" t="s">
-        <v>649</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>650</v>
+      </c>
+      <c r="E11" t="s">
         <v>654</v>
       </c>
-      <c r="D11" t="s">
-        <v>651</v>
-      </c>
-      <c r="E11" t="s">
-        <v>655</v>
-      </c>
       <c r="F11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>655</v>
+      </c>
+      <c r="B12" t="s">
         <v>656</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>657</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>658</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>659</v>
       </c>
-      <c r="E12" t="s">
-        <v>660</v>
-      </c>
       <c r="F12" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -5414,106 +5414,106 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B1" t="s">
         <v>661</v>
-      </c>
-      <c r="B1" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>662</v>
+      </c>
+      <c r="B2" t="s">
         <v>663</v>
-      </c>
-      <c r="B2" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>664</v>
+      </c>
+      <c r="B3" t="s">
         <v>665</v>
-      </c>
-      <c r="B3" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>666</v>
+      </c>
+      <c r="B4" t="s">
         <v>667</v>
-      </c>
-      <c r="B4" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>668</v>
+      </c>
+      <c r="B5" t="s">
         <v>669</v>
-      </c>
-      <c r="B5" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>670</v>
+      </c>
+      <c r="B6" t="s">
         <v>671</v>
-      </c>
-      <c r="B6" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>672</v>
+      </c>
+      <c r="B7" t="s">
         <v>673</v>
-      </c>
-      <c r="B7" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>674</v>
+      </c>
+      <c r="B8" t="s">
         <v>675</v>
-      </c>
-      <c r="B8" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>676</v>
+      </c>
+      <c r="B9" t="s">
         <v>677</v>
-      </c>
-      <c r="B9" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>678</v>
+      </c>
+      <c r="B10" t="s">
         <v>679</v>
-      </c>
-      <c r="B10" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>680</v>
+      </c>
+      <c r="B11" t="s">
         <v>681</v>
-      </c>
-      <c r="B11" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>682</v>
+      </c>
+      <c r="B12" t="s">
         <v>683</v>
-      </c>
-      <c r="B12" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>684</v>
+      </c>
+      <c r="B13" t="s">
         <v>685</v>
-      </c>
-      <c r="B13" t="s">
-        <v>686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>